<commit_message>
Updated the README.md with instructions for how to use this repository moving forward (post the Live session). Added Live_session_Part1.Rmd along with corresponding result graphs and modifications to the mice data for those who want to see exactly what we walked through. Addedadditional_resources/ and additional_resources/extra/ and filled with links and documents that will be useful for people trying to learn
</commit_message>
<xml_diff>
--- a/data/part1/mice.xlsx
+++ b/data/part1/mice.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/tnukols_emory_edu/Documents/Documents/Emory/Clubs_Involvement/DVAC/DVAC_Nov_2020_intro_R_and_ggplot/data/part1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_D84C5477C3574A1C1801C015FCA37DCB2C67D1EF" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F84E3D1A-2AF7-4CBF-B652-D560ADEB5D6D}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -233,13 +241,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -251,7 +256,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -266,24 +271,338 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -306,7 +625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -316,23 +635,23 @@
       <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>6.32</v>
       </c>
-      <c r="E2" t="n" s="2">
-        <v>44117.0</v>
-      </c>
-      <c r="F2" t="n" s="2">
-        <v>44138.0</v>
+      <c r="E2" s="1">
+        <v>44117</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44138</v>
       </c>
       <c r="G2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -342,23 +661,23 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>11.88</v>
       </c>
-      <c r="E3" t="n" s="2">
-        <v>44110.0</v>
-      </c>
-      <c r="F3" t="n" s="2">
-        <v>44131.0</v>
+      <c r="E3" s="1">
+        <v>44110</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44131</v>
       </c>
       <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="H3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -368,23 +687,23 @@
       <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>16.12</v>
       </c>
-      <c r="E4" t="n" s="2">
-        <v>44106.0</v>
-      </c>
-      <c r="F4" t="n" s="2">
-        <v>44127.0</v>
+      <c r="E4" s="1">
+        <v>44106</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44127</v>
       </c>
       <c r="G4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>1.07</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -394,23 +713,23 @@
       <c r="C5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>15.94</v>
       </c>
-      <c r="E5" t="n" s="2">
-        <v>44105.0</v>
-      </c>
-      <c r="F5" t="n" s="2">
-        <v>44126.0</v>
+      <c r="E5" s="1">
+        <v>44105</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44126</v>
       </c>
       <c r="G5" t="s">
         <v>71</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>1.21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -420,23 +739,23 @@
       <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="D6" t="n">
-        <v>17.19</v>
-      </c>
-      <c r="E6" t="n" s="2">
-        <v>44104.0</v>
-      </c>
-      <c r="F6" t="n" s="2">
-        <v>44125.0</v>
+      <c r="D6">
+        <v>17.190000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44104</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44125</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -446,23 +765,23 @@
       <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>19.59</v>
       </c>
-      <c r="E7" t="n" s="2">
-        <v>44090.0</v>
-      </c>
-      <c r="F7" t="n" s="2">
-        <v>44111.0</v>
+      <c r="E7" s="1">
+        <v>44090</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44111</v>
       </c>
       <c r="G7" t="s">
         <v>69</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>1.25</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -472,23 +791,23 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="n">
-        <v>17.65</v>
-      </c>
-      <c r="E8" t="n" s="2">
-        <v>44086.0</v>
-      </c>
-      <c r="F8" t="n" s="2">
-        <v>44107.0</v>
+      <c r="D8">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44086</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44107</v>
       </c>
       <c r="G8" t="s">
         <v>70</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>0.13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -498,23 +817,23 @@
       <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" t="n">
-        <v>19.94</v>
-      </c>
-      <c r="E9" t="n" s="2">
-        <v>44082.0</v>
-      </c>
-      <c r="F9" t="n" s="2">
-        <v>44103.0</v>
+      <c r="D9">
+        <v>19.940000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44082</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44103</v>
       </c>
       <c r="G9" t="s">
         <v>69</v>
       </c>
-      <c r="H9" t="n">
-        <v>1.11</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="H9">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -524,23 +843,23 @@
       <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>20.82</v>
       </c>
-      <c r="E10" t="n" s="2">
-        <v>44078.0</v>
-      </c>
-      <c r="F10" t="n" s="2">
-        <v>44099.0</v>
+      <c r="E10" s="1">
+        <v>44078</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44099</v>
       </c>
       <c r="G10" t="s">
         <v>69</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>1.2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -550,23 +869,23 @@
       <c r="C11" t="s">
         <v>67</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>19.79</v>
       </c>
-      <c r="E11" t="n" s="2">
-        <v>44072.0</v>
-      </c>
-      <c r="F11" t="n" s="2">
-        <v>44093.0</v>
+      <c r="E11" s="1">
+        <v>44072</v>
+      </c>
+      <c r="F11" s="1">
+        <v>44093</v>
       </c>
       <c r="G11" t="s">
         <v>70</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>0.23</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -576,23 +895,23 @@
       <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>20.43</v>
       </c>
-      <c r="E12" t="n" s="2">
-        <v>44068.0</v>
-      </c>
-      <c r="F12" t="n" s="2">
-        <v>44089.0</v>
+      <c r="E12" s="1">
+        <v>44068</v>
+      </c>
+      <c r="F12" s="1">
+        <v>44089</v>
       </c>
       <c r="G12" t="s">
         <v>71</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>0.72</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -602,23 +921,23 @@
       <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>20.79</v>
       </c>
-      <c r="E13" t="n" s="2">
-        <v>44056.0</v>
-      </c>
-      <c r="F13" t="n" s="2">
-        <v>44077.0</v>
+      <c r="E13" s="1">
+        <v>44056</v>
+      </c>
+      <c r="F13" s="1">
+        <v>44077</v>
       </c>
       <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>0.54</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -628,23 +947,23 @@
       <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>21.33</v>
       </c>
-      <c r="E14" t="n" s="2">
-        <v>44049.0</v>
-      </c>
-      <c r="F14" t="n" s="2">
-        <v>44070.0</v>
+      <c r="E14" s="1">
+        <v>44049</v>
+      </c>
+      <c r="F14" s="1">
+        <v>44070</v>
       </c>
       <c r="G14" t="s">
         <v>70</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>0.23</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -654,23 +973,23 @@
       <c r="C15" t="s">
         <v>67</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>21.54</v>
       </c>
-      <c r="E15" t="n" s="2">
-        <v>44044.0</v>
-      </c>
-      <c r="F15" t="n" s="2">
-        <v>44065.0</v>
+      <c r="E15" s="1">
+        <v>44044</v>
+      </c>
+      <c r="F15" s="1">
+        <v>44065</v>
       </c>
       <c r="G15" t="s">
         <v>71</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>0.75</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -680,23 +999,23 @@
       <c r="C16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>21.62</v>
       </c>
-      <c r="E16" t="n" s="2">
-        <v>44044.0</v>
-      </c>
-      <c r="F16" t="n" s="2">
-        <v>44065.0</v>
+      <c r="E16" s="1">
+        <v>44044</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44065</v>
       </c>
       <c r="G16" t="s">
         <v>70</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>0.21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -706,23 +1025,23 @@
       <c r="C17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>22.29</v>
       </c>
-      <c r="E17" t="n" s="2">
-        <v>44029.0</v>
-      </c>
-      <c r="F17" t="n" s="2">
-        <v>44050.0</v>
+      <c r="E17" s="1">
+        <v>44029</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44050</v>
       </c>
       <c r="G17" t="s">
         <v>70</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>0.05</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -732,23 +1051,23 @@
       <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>24.6</v>
       </c>
-      <c r="E18" t="n" s="2">
-        <v>44029.0</v>
-      </c>
-      <c r="F18" t="n" s="2">
-        <v>44050.0</v>
+      <c r="E18" s="1">
+        <v>44029</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44050</v>
       </c>
       <c r="G18" t="s">
         <v>69</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>0.97</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -758,23 +1077,23 @@
       <c r="C19" t="s">
         <v>67</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>22.55</v>
       </c>
-      <c r="E19" t="n" s="2">
-        <v>44021.0</v>
-      </c>
-      <c r="F19" t="n" s="2">
-        <v>44042.0</v>
+      <c r="E19" s="1">
+        <v>44021</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44042</v>
       </c>
       <c r="G19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>0.47</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -784,23 +1103,23 @@
       <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>25.25</v>
       </c>
-      <c r="E20" t="n" s="2">
-        <v>44012.0</v>
-      </c>
-      <c r="F20" t="n" s="2">
-        <v>44033.0</v>
+      <c r="E20" s="1">
+        <v>44012</v>
+      </c>
+      <c r="F20" s="1">
+        <v>44033</v>
       </c>
       <c r="G20" t="s">
         <v>69</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>0.68</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -810,23 +1129,23 @@
       <c r="C21" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>25.59</v>
       </c>
-      <c r="E21" t="n" s="2">
-        <v>44006.0</v>
-      </c>
-      <c r="F21" t="n" s="2">
-        <v>44027.0</v>
+      <c r="E21" s="1">
+        <v>44006</v>
+      </c>
+      <c r="F21" s="1">
+        <v>44027</v>
       </c>
       <c r="G21" t="s">
         <v>69</v>
       </c>
-      <c r="H21" t="n">
-        <v>1.12</v>
-      </c>
-    </row>
-    <row r="22">
+      <c r="H21">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -836,23 +1155,23 @@
       <c r="C22" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>26.08</v>
       </c>
-      <c r="E22" t="n" s="2">
-        <v>43997.0</v>
-      </c>
-      <c r="F22" t="n" s="2">
-        <v>44018.0</v>
+      <c r="E22" s="1">
+        <v>43997</v>
+      </c>
+      <c r="F22" s="1">
+        <v>44018</v>
       </c>
       <c r="G22" t="s">
         <v>69</v>
       </c>
-      <c r="H22" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -862,23 +1181,23 @@
       <c r="C23" t="s">
         <v>67</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>26.18</v>
       </c>
-      <c r="E23" t="n" s="2">
-        <v>43990.0</v>
-      </c>
-      <c r="F23" t="n" s="2">
-        <v>44011.0</v>
+      <c r="E23" s="1">
+        <v>43990</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44011</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>1.06</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -888,23 +1207,23 @@
       <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>24.28</v>
       </c>
-      <c r="E24" t="n" s="2">
-        <v>43990.0</v>
-      </c>
-      <c r="F24" t="n" s="2">
-        <v>44011.0</v>
+      <c r="E24" s="1">
+        <v>43990</v>
+      </c>
+      <c r="F24" s="1">
+        <v>44011</v>
       </c>
       <c r="G24" t="s">
         <v>71</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>0.97</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -914,23 +1233,23 @@
       <c r="C25" t="s">
         <v>67</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>25.21</v>
       </c>
-      <c r="E25" t="n" s="2">
-        <v>43975.0</v>
-      </c>
-      <c r="F25" t="n" s="2">
-        <v>43996.0</v>
+      <c r="E25" s="1">
+        <v>43975</v>
+      </c>
+      <c r="F25" s="1">
+        <v>43996</v>
       </c>
       <c r="G25" t="s">
         <v>70</v>
       </c>
-      <c r="H25" t="n">
-        <v>0.29</v>
-      </c>
-    </row>
-    <row r="26">
+      <c r="H25">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -940,23 +1259,23 @@
       <c r="C26" t="s">
         <v>67</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>26.61</v>
       </c>
-      <c r="E26" t="n" s="2">
-        <v>43972.0</v>
-      </c>
-      <c r="F26" t="n" s="2">
-        <v>43993.0</v>
+      <c r="E26" s="1">
+        <v>43972</v>
+      </c>
+      <c r="F26" s="1">
+        <v>43993</v>
       </c>
       <c r="G26" t="s">
         <v>70</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>0.36</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -966,23 +1285,23 @@
       <c r="C27" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>30.1</v>
       </c>
-      <c r="E27" t="n" s="2">
-        <v>43960.0</v>
-      </c>
-      <c r="F27" t="n" s="2">
-        <v>43981.0</v>
+      <c r="E27" s="1">
+        <v>43960</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43981</v>
       </c>
       <c r="G27" t="s">
         <v>71</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27">
         <v>0.83</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -992,23 +1311,23 @@
       <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>31.47</v>
       </c>
-      <c r="E28" t="n" s="2">
-        <v>43955.0</v>
-      </c>
-      <c r="F28" t="n" s="2">
-        <v>43976.0</v>
+      <c r="E28" s="1">
+        <v>43955</v>
+      </c>
+      <c r="F28" s="1">
+        <v>43976</v>
       </c>
       <c r="G28" t="s">
         <v>71</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28">
         <v>0.82</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1018,23 +1337,23 @@
       <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="D29" t="n">
-        <v>16.83</v>
-      </c>
-      <c r="E29" t="n" s="2">
-        <v>44117.0</v>
-      </c>
-      <c r="F29" t="n" s="2">
-        <v>44138.0</v>
+      <c r="D29">
+        <v>16.829999999999998</v>
+      </c>
+      <c r="E29" s="1">
+        <v>44117</v>
+      </c>
+      <c r="F29" s="1">
+        <v>44138</v>
       </c>
       <c r="G29" t="s">
         <v>71</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>0.77</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1044,23 +1363,23 @@
       <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>24.31</v>
       </c>
-      <c r="E30" t="n" s="2">
-        <v>44110.0</v>
-      </c>
-      <c r="F30" t="n" s="2">
-        <v>44131.0</v>
+      <c r="E30" s="1">
+        <v>44110</v>
+      </c>
+      <c r="F30" s="1">
+        <v>44131</v>
       </c>
       <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30">
         <v>1.32</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1070,23 +1389,23 @@
       <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>25.37</v>
       </c>
-      <c r="E31" t="n" s="2">
-        <v>44110.0</v>
-      </c>
-      <c r="F31" t="n" s="2">
-        <v>44131.0</v>
+      <c r="E31" s="1">
+        <v>44110</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44131</v>
       </c>
       <c r="G31" t="s">
         <v>69</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31">
         <v>1.22</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1096,23 +1415,23 @@
       <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>23.48</v>
       </c>
-      <c r="E32" t="n" s="2">
-        <v>44105.0</v>
-      </c>
-      <c r="F32" t="n" s="2">
-        <v>44126.0</v>
+      <c r="E32" s="1">
+        <v>44105</v>
+      </c>
+      <c r="F32" s="1">
+        <v>44126</v>
       </c>
       <c r="G32" t="s">
         <v>70</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32">
         <v>0.3</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1122,23 +1441,23 @@
       <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>24.25</v>
       </c>
-      <c r="E33" t="n" s="2">
-        <v>44104.0</v>
-      </c>
-      <c r="F33" t="n" s="2">
-        <v>44125.0</v>
+      <c r="E33" s="1">
+        <v>44104</v>
+      </c>
+      <c r="F33" s="1">
+        <v>44125</v>
       </c>
       <c r="G33" t="s">
         <v>71</v>
       </c>
-      <c r="H33" t="n">
-        <v>0.57</v>
-      </c>
-    </row>
-    <row r="34">
+      <c r="H33">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1148,23 +1467,23 @@
       <c r="C34" t="s">
         <v>68</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>24.56</v>
       </c>
-      <c r="E34" t="n" s="2">
-        <v>44092.0</v>
-      </c>
-      <c r="F34" t="n" s="2">
-        <v>44113.0</v>
+      <c r="E34" s="1">
+        <v>44092</v>
+      </c>
+      <c r="F34" s="1">
+        <v>44113</v>
       </c>
       <c r="G34" t="s">
         <v>70</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34">
         <v>0.42</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1174,23 +1493,23 @@
       <c r="C35" t="s">
         <v>68</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>26.96</v>
       </c>
-      <c r="E35" t="n" s="2">
-        <v>44090.0</v>
-      </c>
-      <c r="F35" t="n" s="2">
-        <v>44111.0</v>
+      <c r="E35" s="1">
+        <v>44090</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44111</v>
       </c>
       <c r="G35" t="s">
         <v>69</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35">
         <v>0.77</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1200,23 +1519,23 @@
       <c r="C36" t="s">
         <v>68</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>24.94</v>
       </c>
-      <c r="E36" t="n" s="2">
-        <v>44086.0</v>
-      </c>
-      <c r="F36" t="n" s="2">
-        <v>44107.0</v>
+      <c r="E36" s="1">
+        <v>44086</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44107</v>
       </c>
       <c r="G36" t="s">
         <v>71</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H36">
         <v>0.96</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1226,23 +1545,23 @@
       <c r="C37" t="s">
         <v>68</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>25.51</v>
       </c>
-      <c r="E37" t="n" s="2">
-        <v>44086.0</v>
-      </c>
-      <c r="F37" t="n" s="2">
-        <v>44107.0</v>
+      <c r="E37" s="1">
+        <v>44086</v>
+      </c>
+      <c r="F37" s="1">
+        <v>44107</v>
       </c>
       <c r="G37" t="s">
         <v>71</v>
       </c>
-      <c r="H37" t="n">
+      <c r="H37">
         <v>0.81</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1252,23 +1571,23 @@
       <c r="C38" t="s">
         <v>68</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>25.99</v>
       </c>
-      <c r="E38" t="n" s="2">
-        <v>44078.0</v>
-      </c>
-      <c r="F38" t="n" s="2">
-        <v>44099.0</v>
+      <c r="E38" s="1">
+        <v>44078</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44099</v>
       </c>
       <c r="G38" t="s">
         <v>71</v>
       </c>
-      <c r="H38" t="n">
+      <c r="H38">
         <v>0.81</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1278,23 +1597,23 @@
       <c r="C39" t="s">
         <v>68</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>27.43</v>
       </c>
-      <c r="E39" t="n" s="2">
-        <v>44072.0</v>
-      </c>
-      <c r="F39" t="n" s="2">
-        <v>44093.0</v>
+      <c r="E39" s="1">
+        <v>44072</v>
+      </c>
+      <c r="F39" s="1">
+        <v>44093</v>
       </c>
       <c r="G39" t="s">
         <v>71</v>
       </c>
-      <c r="H39" t="n">
+      <c r="H39">
         <v>1.05</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1304,23 +1623,23 @@
       <c r="C40" t="s">
         <v>68</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>28.33</v>
       </c>
-      <c r="E40" t="n" s="2">
-        <v>44054.0</v>
-      </c>
-      <c r="F40" t="n" s="2">
-        <v>44075.0</v>
+      <c r="E40" s="1">
+        <v>44054</v>
+      </c>
+      <c r="F40" s="1">
+        <v>44075</v>
       </c>
       <c r="G40" t="s">
         <v>71</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H40">
         <v>0.81</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1330,23 +1649,23 @@
       <c r="C41" t="s">
         <v>68</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>28.87</v>
       </c>
-      <c r="E41" t="n" s="2">
-        <v>44047.0</v>
-      </c>
-      <c r="F41" t="n" s="2">
-        <v>44068.0</v>
+      <c r="E41" s="1">
+        <v>44047</v>
+      </c>
+      <c r="F41" s="1">
+        <v>44068</v>
       </c>
       <c r="G41" t="s">
         <v>70</v>
       </c>
-      <c r="H41" t="n">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="42">
+      <c r="H41">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1356,23 +1675,23 @@
       <c r="C42" t="s">
         <v>68</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>28.97</v>
       </c>
-      <c r="E42" t="n" s="2">
-        <v>44044.0</v>
-      </c>
-      <c r="F42" t="n" s="2">
-        <v>44065.0</v>
+      <c r="E42" s="1">
+        <v>44044</v>
+      </c>
+      <c r="F42" s="1">
+        <v>44065</v>
       </c>
       <c r="G42" t="s">
         <v>71</v>
       </c>
-      <c r="H42" t="n">
+      <c r="H42">
         <v>0.84</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1382,23 +1701,23 @@
       <c r="C43" t="s">
         <v>68</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>29.2</v>
       </c>
-      <c r="E43" t="n" s="2">
-        <v>44033.0</v>
-      </c>
-      <c r="F43" t="n" s="2">
-        <v>44054.0</v>
+      <c r="E43" s="1">
+        <v>44033</v>
+      </c>
+      <c r="F43" s="1">
+        <v>44054</v>
       </c>
       <c r="G43" t="s">
         <v>71</v>
       </c>
-      <c r="H43" t="n">
-        <v>1.16</v>
-      </c>
-    </row>
-    <row r="44">
+      <c r="H43">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1408,23 +1727,23 @@
       <c r="C44" t="s">
         <v>68</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>29.3</v>
       </c>
-      <c r="E44" t="n" s="2">
-        <v>44029.0</v>
-      </c>
-      <c r="F44" t="n" s="2">
-        <v>44050.0</v>
+      <c r="E44" s="1">
+        <v>44029</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44050</v>
       </c>
       <c r="G44" t="s">
         <v>70</v>
       </c>
-      <c r="H44" t="n">
+      <c r="H44">
         <v>0.27</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1434,23 +1753,23 @@
       <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>29.32</v>
       </c>
-      <c r="E45" t="n" s="2">
-        <v>44027.0</v>
-      </c>
-      <c r="F45" t="n" s="2">
-        <v>44048.0</v>
+      <c r="E45" s="1">
+        <v>44027</v>
+      </c>
+      <c r="F45" s="1">
+        <v>44048</v>
       </c>
       <c r="G45" t="s">
         <v>70</v>
       </c>
-      <c r="H45" t="n">
+      <c r="H45">
         <v>0.45</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1460,23 +1779,23 @@
       <c r="C46" t="s">
         <v>68</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>32.68</v>
       </c>
-      <c r="E46" t="n" s="2">
-        <v>44025.0</v>
-      </c>
-      <c r="F46" t="n" s="2">
-        <v>44046.0</v>
+      <c r="E46" s="1">
+        <v>44025</v>
+      </c>
+      <c r="F46" s="1">
+        <v>44046</v>
       </c>
       <c r="G46" t="s">
         <v>69</v>
       </c>
-      <c r="H46" t="n">
+      <c r="H46">
         <v>1.24</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1486,23 +1805,23 @@
       <c r="C47" t="s">
         <v>68</v>
       </c>
-      <c r="D47" t="n">
-        <v>32.73</v>
-      </c>
-      <c r="E47" t="n" s="2">
-        <v>44021.0</v>
-      </c>
-      <c r="F47" t="n" s="2">
-        <v>44042.0</v>
+      <c r="D47">
+        <v>32.729999999999997</v>
+      </c>
+      <c r="E47" s="1">
+        <v>44021</v>
+      </c>
+      <c r="F47" s="1">
+        <v>44042</v>
       </c>
       <c r="G47" t="s">
         <v>69</v>
       </c>
-      <c r="H47" t="n">
+      <c r="H47">
         <v>1.19</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1512,23 +1831,23 @@
       <c r="C48" t="s">
         <v>68</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>30.67</v>
       </c>
-      <c r="E48" t="n" s="2">
-        <v>44012.0</v>
-      </c>
-      <c r="F48" t="n" s="2">
-        <v>44033.0</v>
+      <c r="E48" s="1">
+        <v>44012</v>
+      </c>
+      <c r="F48" s="1">
+        <v>44033</v>
       </c>
       <c r="G48" t="s">
         <v>70</v>
       </c>
-      <c r="H48" t="n">
+      <c r="H48">
         <v>0.25</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1538,23 +1857,23 @@
       <c r="C49" t="s">
         <v>68</v>
       </c>
-      <c r="D49" t="n">
-        <v>33.12</v>
-      </c>
-      <c r="E49" t="n" s="2">
-        <v>44010.0</v>
-      </c>
-      <c r="F49" t="n" s="2">
-        <v>44031.0</v>
+      <c r="D49">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="E49" s="1">
+        <v>44010</v>
+      </c>
+      <c r="F49" s="1">
+        <v>44031</v>
       </c>
       <c r="G49" t="s">
         <v>69</v>
       </c>
-      <c r="H49" t="n">
-        <v>1.11</v>
-      </c>
-    </row>
-    <row r="50">
+      <c r="H49">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1564,23 +1883,23 @@
       <c r="C50" t="s">
         <v>68</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>31.22</v>
       </c>
-      <c r="E50" t="n" s="2">
-        <v>43997.0</v>
-      </c>
-      <c r="F50" t="n" s="2">
-        <v>44018.0</v>
+      <c r="E50" s="1">
+        <v>43997</v>
+      </c>
+      <c r="F50" s="1">
+        <v>44018</v>
       </c>
       <c r="G50" t="s">
         <v>71</v>
       </c>
-      <c r="H50" t="n">
+      <c r="H50">
         <v>1.05</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1590,23 +1909,23 @@
       <c r="C51" t="s">
         <v>68</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>33.74</v>
       </c>
-      <c r="E51" t="n" s="2">
-        <v>43990.0</v>
-      </c>
-      <c r="F51" t="n" s="2">
-        <v>44011.0</v>
+      <c r="E51" s="1">
+        <v>43990</v>
+      </c>
+      <c r="F51" s="1">
+        <v>44011</v>
       </c>
       <c r="G51" t="s">
         <v>69</v>
       </c>
-      <c r="H51" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="52">
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -1616,23 +1935,23 @@
       <c r="C52" t="s">
         <v>68</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>35.96</v>
       </c>
-      <c r="E52" t="n" s="2">
-        <v>43990.0</v>
-      </c>
-      <c r="F52" t="n" s="2">
-        <v>44011.0</v>
+      <c r="E52" s="1">
+        <v>43990</v>
+      </c>
+      <c r="F52" s="1">
+        <v>44011</v>
       </c>
       <c r="G52" t="s">
         <v>69</v>
       </c>
-      <c r="H52" t="n">
+      <c r="H52">
         <v>1.22</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1642,23 +1961,23 @@
       <c r="C53" t="s">
         <v>68</v>
       </c>
-      <c r="D53" t="n">
-        <v>33.7</v>
-      </c>
-      <c r="E53" t="n" s="2">
-        <v>43984.0</v>
-      </c>
-      <c r="F53" t="n" s="2">
-        <v>44005.0</v>
+      <c r="D53">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E53" s="1">
+        <v>43984</v>
+      </c>
+      <c r="F53" s="1">
+        <v>44005</v>
       </c>
       <c r="G53" t="s">
         <v>70</v>
       </c>
-      <c r="H53" t="n">
+      <c r="H53">
         <v>0.22</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -1668,23 +1987,23 @@
       <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>34.39</v>
       </c>
-      <c r="E54" t="n" s="2">
-        <v>43984.0</v>
-      </c>
-      <c r="F54" t="n" s="2">
-        <v>44005.0</v>
+      <c r="E54" s="1">
+        <v>43984</v>
+      </c>
+      <c r="F54" s="1">
+        <v>44005</v>
       </c>
       <c r="G54" t="s">
         <v>71</v>
       </c>
-      <c r="H54" t="n">
+      <c r="H54">
         <v>0.77</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1694,23 +2013,23 @@
       <c r="C55" t="s">
         <v>68</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>34.42</v>
       </c>
-      <c r="E55" t="n" s="2">
-        <v>43982.0</v>
-      </c>
-      <c r="F55" t="n" s="2">
-        <v>44003.0</v>
+      <c r="E55" s="1">
+        <v>43982</v>
+      </c>
+      <c r="F55" s="1">
+        <v>44003</v>
       </c>
       <c r="G55" t="s">
         <v>70</v>
       </c>
-      <c r="H55" t="n">
+      <c r="H55">
         <v>0.06</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -1720,23 +2039,23 @@
       <c r="C56" t="s">
         <v>68</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>34.43</v>
       </c>
-      <c r="E56" t="n" s="2">
-        <v>43972.0</v>
-      </c>
-      <c r="F56" t="n" s="2">
-        <v>43993.0</v>
+      <c r="E56" s="1">
+        <v>43972</v>
+      </c>
+      <c r="F56" s="1">
+        <v>43993</v>
       </c>
       <c r="G56" t="s">
         <v>71</v>
       </c>
-      <c r="H56" t="n">
+      <c r="H56">
         <v>0.79</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -1746,23 +2065,23 @@
       <c r="C57" t="s">
         <v>68</v>
       </c>
-      <c r="D57" t="n">
-        <v>34.87</v>
-      </c>
-      <c r="E57" t="n" s="2">
-        <v>43960.0</v>
-      </c>
-      <c r="F57" t="n" s="2">
-        <v>43981.0</v>
+      <c r="D57">
+        <v>34.869999999999997</v>
+      </c>
+      <c r="E57" s="1">
+        <v>43960</v>
+      </c>
+      <c r="F57" s="1">
+        <v>43981</v>
       </c>
       <c r="G57" t="s">
         <v>71</v>
       </c>
-      <c r="H57" t="n">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="58">
+      <c r="H57">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -1772,23 +2091,23 @@
       <c r="C58" t="s">
         <v>68</v>
       </c>
-      <c r="D58" t="n">
-        <v>35.91</v>
-      </c>
-      <c r="E58" t="n" s="2">
-        <v>43955.0</v>
-      </c>
-      <c r="F58" t="n" s="2">
-        <v>43976.0</v>
+      <c r="D58">
+        <v>35.909999999999997</v>
+      </c>
+      <c r="E58" s="1">
+        <v>43955</v>
+      </c>
+      <c r="F58" s="1">
+        <v>43976</v>
       </c>
       <c r="G58" t="s">
         <v>70</v>
       </c>
-      <c r="H58" t="n">
+      <c r="H58">
         <v>0.31</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -1798,23 +2117,23 @@
       <c r="C59" t="s">
         <v>68</v>
       </c>
-      <c r="D59" t="n">
-        <v>38.23</v>
-      </c>
-      <c r="E59" t="n" s="2">
-        <v>43954.0</v>
-      </c>
-      <c r="F59" t="n" s="2">
-        <v>43975.0</v>
+      <c r="D59">
+        <v>38.229999999999997</v>
+      </c>
+      <c r="E59" s="1">
+        <v>43954</v>
+      </c>
+      <c r="F59" s="1">
+        <v>43975</v>
       </c>
       <c r="G59" t="s">
         <v>69</v>
       </c>
-      <c r="H59" t="n">
-        <v>1.15</v>
-      </c>
-    </row>
-    <row r="60">
+      <c r="H59">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -1824,23 +2143,23 @@
       <c r="C60" t="s">
         <v>68</v>
       </c>
-      <c r="D60" t="n">
-        <v>38.98</v>
-      </c>
-      <c r="E60" t="n" s="2">
-        <v>43943.0</v>
-      </c>
-      <c r="F60" t="n" s="2">
-        <v>43964.0</v>
+      <c r="D60">
+        <v>38.979999999999997</v>
+      </c>
+      <c r="E60" s="1">
+        <v>43943</v>
+      </c>
+      <c r="F60" s="1">
+        <v>43964</v>
       </c>
       <c r="G60" t="s">
         <v>69</v>
       </c>
-      <c r="H60" t="n">
+      <c r="H60">
         <v>1.08</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -1850,23 +2169,23 @@
       <c r="C61" t="s">
         <v>68</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61">
         <v>36.89</v>
       </c>
-      <c r="E61" t="n" s="2">
-        <v>43943.0</v>
-      </c>
-      <c r="F61" t="n" s="2">
-        <v>43964.0</v>
+      <c r="E61" s="1">
+        <v>43943</v>
+      </c>
+      <c r="F61" s="1">
+        <v>43964</v>
       </c>
       <c r="G61" t="s">
         <v>71</v>
       </c>
-      <c r="H61" t="n">
+      <c r="H61">
         <v>1.71</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>